<commit_message>
Augment and style the research summary for the qualification.
</commit_message>
<xml_diff>
--- a/gaiyou-ie-daigakuinshinsa.xlsx
+++ b/gaiyou-ie-daigakuinshinsa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sato\wsl\home\sato\paper\cv2023_uec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB075143-D70E-448E-8F96-EF024AF5BCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E851C6C7-9DE8-4597-B15B-908B78DC8491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t>単著・
 共著の別</t>
@@ -475,11 +475,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t xml:space="preserve">並列および並行プログラミングでは，カーネルレベルスレッドに不足している効率的で柔軟な機能を提供するユーザーレベルスレッドが有用であり，それを提供するシステムが長く開発されてきている．しかし，既存システムのほとんどは，カスタマイズに追加コストが発生するモノリシックライブラリとして実装されている．本研究では，C++の抽象化を用いて，インターフェイス・コストを最小限に抑えながら高いカスタマイズ性を提供する新しいユーザレベルスレッドライブラリを開発した．
-</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>グラフデータの増大に伴い，大規模入力に対してスケーラブルな分散グラフ処理システムが活発に研究されており，最先端の分散グラフ処理システムGeminiでは，軽量なグラフ分割や負荷分散を用いることで，スケーラビリティと効率の両立を達成している．しかし，グラフを一般化したハイパーグラフに関する処理系の研究はあまり進んでおらず，ハイパーグラフ処理におけるスケーラビリティと効率の両立は未解決の課題である．本研究では，Geminiをベースとして，スケーラビリティと効率性を両立する分散ハイパーグラフ処理システムを開発し，その性能を評価した．</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -525,6 +520,106 @@
   </si>
   <si>
     <t>条件分岐を伴う複雑な漸化式やリスト走査の並列化は，主に形式化に焦点を置いた理論研究において扱われてきた．一方，実際のプログラムに対する自動並列化を扱うコンパイラには，その理論的成果が取り込まれておらず，データ依存がある場合については，総和などの単純なパターンを抽出して，アドホックに並列化することに留まっている．そこで本研究では，並列化の理論と実装ギャップを埋めるために，複雑なリダクションを扱うことができる行列乗算による並列化を，コンパイラ技術として取り込む実装技法を開発した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>並列および並行プログラミングでは，カーネルレベルスレッドに不足している効率的で柔軟な機能を提供するユーザーレベルスレッドが有用であり，それを提供するシステムが長く開発されてきている．しかし，既存システムのほとんどは，カスタマイズに追加コストが発生するモノリシックライブラリとして実装されている．本研究では，C++の抽象化を用いて，インターフェイス・コストを最小限に抑えながら高いカスタマイズ性を提供する新しいユーザレベルスレッドライブラリを開発した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>4 Pitfalls of InfiniBand with On-Demand Paging.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ISPASS 2021</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>5 MENPS: A Decentralized Distributed Shared Memory Exploiting RDMA.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>IPDRM 2020</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>6 Parallelization of XPath Queries using Modern XQuery Processors.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ADBIS 2018</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>7 A Debugger-Cooperative Higher-Order Contract System in Python.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>8 s6raph: Vertex-Centric Graph Processing Framework with Functional Interface.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>APLAS 2016</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>FHPC 2016</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>GPCE 2015</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>APLAS 2014</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>13 A Skeletal Parallel Framework with Fusion Optimizer for GPGPU Programming.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>11 Syntax-Directed Divide-and-Conquer Data-Flow Analysis.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>10 LibDSL: A Library for Developing Embedded Domain Specific Languages in D via Template Metaprogramming.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>APLAS 2009</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>普及した高性能ネットワーク規格であるInfiniBandは，OSを迂回した低遅延通信であるRDMA（Remote Direct Memory Access）が可能であり，その新たな拡張機能であるオンデマンドページング（ODP）では，RDMA由来のページフォルトによるメモリ管理が可能になっている．既存研究では，ODPのオーバーヘッドが十分に小さいと報告されているが，再送やタイムアウトを含む様々なネットワーク状況での調査は不足している．本研究では、さまざまなデバイス上でのODPの実際の動作について包括的な分析を行い，通常のページフォルトよりも3～4桁長い待ち時間が発生する状況を発見した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>RDMA（Remote Direct Memory Access)に対応したネットワークデバイスの普及により，通信を担うミドルウェアについて，RDMAを前提とした新しい設計オプションを模索することができる状況になった．本研究では， 複数の計算ノードにまたがる共有メモリを提供する分散共有メモリ（DSM）のソフトウェア実装に焦点を当て，RDMAに適したDSMのための通信手法を設計し，それを用いたDSMライブラリMENPSを開発した．MENPSは，最先端のRDMAに基づくDSMシステムを上回る実験性能を示した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>XMLデータベースに対するクエリ言語であるXPathを並列化する実用的で有望なアプローチを，2009年にBordawekarらが提案した．彼らのアプローチは，既存のXMLデータベースエンジン上での並列化を可能にするものであり，彼らはそれによる速度向上を実験的に示した．しかし，XMLクエリ言語の処理能力向上に伴ってソフトウェア環境が大きく変化したため，彼らの実践は既に時代遅れとなっている．本研究では，最先端のXMLデータベースエンジンの上で，彼らのアプローチを2通りの方法で実装し，一般的なサーバ上で大幅な高速化が可能であることを実験的に示した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>契約プログラミングは，Pythonのような動的な自由度が大きいプログラミング言語の信頼性を向上させる最も有望な方法の1つであり，Pythonへの適用が有望であるが，Pythonにおけるイテレータや関数の振る舞いを完全に指定できる高階契約システムはまだない．また，高階契約検査は必要になるまで遅延されるため，副作用が多いPythonでは，契約違反が起きた際のデバッグ負担が大きい．この問題を解決するために、Pythonの高階契約システムPyBlameと遅延契約検査のデバッグに特化した機能を備えたソースレベルデバッガccdbを開発した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ビッグデータ処理の文脈において，グラフの並列分散処理の需要は大きく，活発に研究されており，Pregelに代表される頂点中心モデルを用いたグラフ処理系が普及してきている．しかし，既存の頂点中心型のグラフ処理系は，アルゴリズム仕様と無関係な副作用や制御文に満ちた可読性の低いコードを，プログラマに書くことを強いるという問題がある．本研究では，プログラマは明確で簡潔な関数を書くことができる関数型インタフェースを備えた，頂点中心型のグラフ処理処理系であるs6raphを開発した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>汎用プログラミング言語に加えて，特定用途特化したドメイン特化言語（DSL）を利用することは，プログラミングの生産性を高めることが知られている．DSLの実装形態として，既存の汎用言語の中でライブラリとして埋め込まれた，埋め込みDSL（EDSL）が採用されることが多い．このEDSLは，埋め込み先の言語を使って全て手作業で記述することが多く，モジュラーに再利用可能な言語処理系構成支援ツールが乏しい．そこで本研究では，与えられた言語仕様から，構文解析器と実行エンジンの両方を機械的に生成する，Ｄ言語向けEDSLの構成支援ライブラリLibDSLを開発した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>現代の最適化コンパイラは，積極的な関数インライン化により，コード最適化に際して大規模なプログラムを扱うのが一般的である．そのため，コード最適化に不可欠な計算であるデータフロー解析（DFA）は、，規模手続きへの対応が望まれている．大規模プログラムのDFAに対する有望なアプローチは，入力プログラムの構文に沿って分解する分割統治型並列化がある．しかし，goto文のような非構造的な制御フローの存在が，構文に沿った分割統治を困難にする．そこで本研究では，非構造的な制御フローを分離しながら，プログラム全体を構文に沿って分割統治を行う並列DFA手法を開発した．</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>GPUの高性能化に伴って，GPU上の汎用コンピューティング（GPGPU）は活発に研究されるようになっているが，GPU上のアプリケーションの開発は，1) 高性能化に並列化と最適化の両方が必要であり，2) 対象アプリケーションがGPUに適しているかどうかを実験的に判断する必要があるという2つの理由により，依然として多大な手間が掛かる．本研究では，並列計算パターン（スケルトン）に基づくGPGPUフレームワークを開発した．提案フレームワークは，スケルトンの合成に対する最適化と，GPU向け実装とCPU向け実装の透過的生成によって，GPGPUプログラミングの手間を削減する．</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -877,6 +972,33 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -901,38 +1023,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1241,40 +1336,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F36"/>
+  <dimension ref="A2:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.21875" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
     <col min="6" max="6" width="55" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="11" t="s">
         <v>11</v>
       </c>
@@ -1292,25 +1387,25 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="35"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="126" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
@@ -1323,12 +1418,12 @@
       <c r="D6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1341,12 +1436,12 @@
       <c r="D7" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E7" s="29"/>
+      <c r="F7" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="154" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1359,12 +1454,12 @@
       <c r="D8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="29"/>
+      <c r="F8" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="126" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1377,12 +1472,12 @@
       <c r="D9" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="E9" s="29"/>
+      <c r="F9" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1395,12 +1490,12 @@
       <c r="D10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="29"/>
+      <c r="F10" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -1413,12 +1508,12 @@
       <c r="D11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="29"/>
+      <c r="F11" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
@@ -1431,12 +1526,12 @@
       <c r="D12" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="29"/>
+      <c r="F12" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="154" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
@@ -1449,12 +1544,12 @@
       <c r="D13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="E13" s="29"/>
+      <c r="F13" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="140" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -1467,80 +1562,80 @@
       <c r="D14" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="13.95" x14ac:dyDescent="0.2">
+      <c r="E14" s="29"/>
+      <c r="F14" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="33"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="13.95" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>1</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="13.95" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>2</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="13.95" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>3</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="13.95" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="154" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>34</v>
       </c>
@@ -1550,15 +1645,15 @@
       <c r="C22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="E22" s="27"/>
+      <c r="F22" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="154" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>35</v>
       </c>
@@ -1568,15 +1663,15 @@
       <c r="C23" s="9">
         <v>2021</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="E23" s="29"/>
+      <c r="F23" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="168" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>36</v>
       </c>
@@ -1586,141 +1681,308 @@
       <c r="C24" s="9">
         <v>2021</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="E24" s="27"/>
+      <c r="F24" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="168" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="9">
+        <v>2021</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="140" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2020</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="154" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="9">
+        <v>2018</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="154" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2018</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="140" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2018</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="27"/>
+      <c r="F29" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="154" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="9">
         <v>2015</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D30" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="6" t="s">
+      <c r="E30" s="27"/>
+      <c r="F30" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="154" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="9">
+        <v>2014</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="27"/>
+      <c r="F31" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="168" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="9">
+        <v>2014</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="27"/>
+      <c r="F32" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="154" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2011</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="27"/>
+      <c r="F33" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="9" t="s">
+    <row r="34" spans="1:6" ht="154" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="9">
-        <v>2011</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="C34" s="9">
+        <v>2014</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="27"/>
+      <c r="F34" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14" x14ac:dyDescent="0.2">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
         <v>1</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" ht="14" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>2</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" ht="14" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
         <v>3</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" ht="14" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="34" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="42" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="39">
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D35:E35"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D24:E24"/>
@@ -1731,24 +1993,9 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1762,7 +2009,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1775,7 +2022,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Style the research summary for the qualification.
</commit_message>
<xml_diff>
--- a/gaiyou-ie-daigakuinshinsa.xlsx
+++ b/gaiyou-ie-daigakuinshinsa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sato\wsl\home\sato\paper\cv2023_uec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E851C6C7-9DE8-4597-B15B-908B78DC8491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AE2F5F-AE21-42A7-B0AD-AD8BB5F7A377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,7 +905,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -942,9 +942,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -975,6 +972,45 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -987,47 +1023,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1338,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1352,28 +1355,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1387,10 +1390,10 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1399,32 +1402,32 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="126" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="9">
         <v>2022</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="22" t="s">
+      <c r="E6" s="32"/>
+      <c r="F6" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="140" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="41" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -1433,16 +1436,16 @@
       <c r="C7" s="9">
         <v>2022</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="22" t="s">
+      <c r="E7" s="32"/>
+      <c r="F7" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1451,16 +1454,16 @@
       <c r="C8" s="9">
         <v>2021</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="22" t="s">
+      <c r="E8" s="32"/>
+      <c r="F8" s="21" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="126" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="41" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1469,16 +1472,16 @@
       <c r="C9" s="9">
         <v>2020</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="32"/>
+      <c r="F9" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="140" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="41" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -1487,16 +1490,16 @@
       <c r="C10" s="9">
         <v>2018</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="140" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="41" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1505,16 +1508,16 @@
       <c r="C11" s="9">
         <v>2017</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="32"/>
+      <c r="F11" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="140" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="41" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1523,16 +1526,16 @@
       <c r="C12" s="9">
         <v>2016</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="22" t="s">
+      <c r="E12" s="32"/>
+      <c r="F12" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="41" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1541,16 +1544,16 @@
       <c r="C13" s="9">
         <v>2015</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="32"/>
+      <c r="F13" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="140" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="41" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1559,11 +1562,11 @@
       <c r="C14" s="9">
         <v>2013</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="22" t="s">
+      <c r="E14" s="32"/>
+      <c r="F14" s="21" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1571,8 +1574,8 @@
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1581,8 +1584,8 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1591,8 +1594,8 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1601,8 +1604,8 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1611,8 +1614,8 @@
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1621,22 +1624,22 @@
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -1645,16 +1648,16 @@
       <c r="C22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="22" t="s">
+      <c r="E22" s="22"/>
+      <c r="F22" s="21" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -1663,16 +1666,16 @@
       <c r="C23" s="9">
         <v>2021</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="22" t="s">
+      <c r="E23" s="32"/>
+      <c r="F23" s="21" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="168" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="41" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -1681,16 +1684,16 @@
       <c r="C24" s="9">
         <v>2021</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="22"/>
+      <c r="F24" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="168" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="41" t="s">
         <v>60</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -1699,16 +1702,16 @@
       <c r="C25" s="9">
         <v>2021</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="22" t="s">
+      <c r="E25" s="22"/>
+      <c r="F25" s="21" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="140" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -1717,16 +1720,16 @@
       <c r="C26" s="9">
         <v>2020</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="22" t="s">
+      <c r="E26" s="22"/>
+      <c r="F26" s="21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="41" t="s">
         <v>64</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -1735,16 +1738,16 @@
       <c r="C27" s="9">
         <v>2018</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="22" t="s">
+      <c r="E27" s="22"/>
+      <c r="F27" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="41" t="s">
         <v>66</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -1753,16 +1756,16 @@
       <c r="C28" s="9">
         <v>2018</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="22" t="s">
+      <c r="E28" s="22"/>
+      <c r="F28" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="140" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="41" t="s">
         <v>67</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -1771,16 +1774,16 @@
       <c r="C29" s="9">
         <v>2018</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="22" t="s">
+      <c r="E29" s="22"/>
+      <c r="F29" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="41" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -1789,16 +1792,16 @@
       <c r="C30" s="9">
         <v>2015</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="22" t="s">
+      <c r="E30" s="22"/>
+      <c r="F30" s="21" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="41" t="s">
         <v>74</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -1807,16 +1810,16 @@
       <c r="C31" s="9">
         <v>2014</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="27"/>
-      <c r="F31" s="22" t="s">
+      <c r="E31" s="22"/>
+      <c r="F31" s="21" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="168" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="41" t="s">
         <v>73</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -1825,16 +1828,16 @@
       <c r="C32" s="9">
         <v>2014</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="22" t="s">
+      <c r="E32" s="22"/>
+      <c r="F32" s="21" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -1843,16 +1846,16 @@
       <c r="C33" s="9">
         <v>2011</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="22" t="s">
+      <c r="E33" s="22"/>
+      <c r="F33" s="21" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="154" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="41" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="9" t="s">
@@ -1861,20 +1864,20 @@
       <c r="C34" s="9">
         <v>2014</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="22" t="s">
+      <c r="E34" s="22"/>
+      <c r="F34" s="21" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1883,8 +1886,8 @@
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1893,8 +1896,8 @@
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1903,8 +1906,8 @@
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1913,8 +1916,8 @@
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:6" ht="14" x14ac:dyDescent="0.2">
@@ -1923,47 +1926,56 @@
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
       <c r="F40" s="8"/>
     </row>
     <row r="42" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="A2:F2"/>
@@ -1980,22 +1992,13 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D31:E31"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>